<commit_message>
Change to git notes
</commit_message>
<xml_diff>
--- a/Git/Git Notes.xlsx
+++ b/Git/Git Notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="20730" windowHeight="10050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>git init</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>Same as above</t>
+  </si>
+  <si>
+    <t>what difference?</t>
   </si>
 </sst>
 </file>
@@ -540,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,9 +694,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
+      </c>
+      <c r="B33" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Git notes for diff
</commit_message>
<xml_diff>
--- a/Git/Git Notes.xlsx
+++ b/Git/Git Notes.xlsx
@@ -150,24 +150,76 @@
     <t xml:space="preserve">removes remote repository refrence to current working directory </t>
   </si>
   <si>
-    <t>update remote repository with local</t>
-  </si>
-  <si>
     <t>git pull origin master</t>
   </si>
   <si>
     <t>Same as above</t>
   </si>
   <si>
-    <t>what is the difference?</t>
+    <t>Shows difference between working directory copy and git repository copy</t>
+  </si>
+  <si>
+    <r>
+      <t>update remote repository with local (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>origin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -&gt; Name of remote repo; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>master</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -&gt; branch on remote repo)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -544,13 +596,13 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="69.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -680,10 +732,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
         <v>45</v>
-      </c>
-      <c r="B25" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -691,7 +743,7 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -699,11 +751,12 @@
         <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
change to inlcude merge
</commit_message>
<xml_diff>
--- a/Git/Git Notes.xlsx
+++ b/Git/Git Notes.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
   <si>
     <t>git init</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>git --merged</t>
+  </si>
+  <si>
+    <t>git merge dev</t>
   </si>
 </sst>
 </file>
@@ -826,7 +829,7 @@
   <dimension ref="A2:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,7 +896,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
Added notes for commands
</commit_message>
<xml_diff>
--- a/Git/Git Notes.xlsx
+++ b/Git/Git Notes.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="20730" windowHeight="10050" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="20730" windowHeight="10050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Branches" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Images" sheetId="3" r:id="rId4"/>
+    <sheet name="Commands" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Images" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="77">
   <si>
     <t>git init</t>
   </si>
@@ -268,6 +269,30 @@
   </si>
   <si>
     <t>git merge dev</t>
+  </si>
+  <si>
+    <t>git checkout Test.txt</t>
+  </si>
+  <si>
+    <t>rolls back changes on Test.txt until previous commit</t>
+  </si>
+  <si>
+    <t>git commit --amend -m "Changed message"</t>
+  </si>
+  <si>
+    <t>to modify previously commited message</t>
+  </si>
+  <si>
+    <t>git commit --amend</t>
+  </si>
+  <si>
+    <t>if you want commit a new file as part of the previous commit</t>
+  </si>
+  <si>
+    <t>git log --stat</t>
+  </si>
+  <si>
+    <t>shows the files commited within each of the previous commits</t>
   </si>
 </sst>
 </file>
@@ -657,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,67 +779,75 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s">
-        <v>38</v>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>28</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>42</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>44</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>33</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>41</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>46</v>
       </c>
     </row>
@@ -828,7 +861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -937,6 +970,57 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -1000,7 +1084,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Changes to MVC Notes
</commit_message>
<xml_diff>
--- a/Git/Git Notes.xlsx
+++ b/Git/Git Notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="20730" windowHeight="10050" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="20730" windowHeight="10050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="109">
   <si>
     <t>git init</t>
   </si>
@@ -430,6 +430,12 @@
   </si>
   <si>
     <t>git stash</t>
+  </si>
+  <si>
+    <t>git push -u origin dev:dev1</t>
+  </si>
+  <si>
+    <t>pushes local dev branch to remote dev1 branch</t>
   </si>
 </sst>
 </file>
@@ -834,7 +840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1009,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B18"/>
+  <dimension ref="A2:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,56 +1067,64 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" t="s">
-        <v>59</v>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>33</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>65</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1123,7 +1137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>

</xml_diff>